<commit_message>
Sending Figs for 1.25 back to laptop for post processing
</commit_message>
<xml_diff>
--- a/ErrorAnalysisNew.xlsx
+++ b/ErrorAnalysisNew.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\MS_MEEN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Fractional_Calculus\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12948" windowHeight="10578" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12945" windowHeight="10575" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="9">
   <si>
     <t>N</t>
   </si>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -300,6 +300,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BA91-4513-9D6F-BA73ADE3B8E3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -389,6 +394,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BA91-4513-9D6F-BA73ADE3B8E3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -478,6 +488,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-BA91-4513-9D6F-BA73ADE3B8E3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -543,7 +558,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -662,7 +676,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1636,7 +1649,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1644,19 +1657,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="I56" sqref="I56:I57"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82:G83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1679,7 +1692,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -1702,7 +1715,7 @@
         <v>7.6554334527432127E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1725,7 +1738,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20</v>
       </c>
@@ -1748,7 +1761,7 @@
         <v>2.4849852095495751E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1771,7 +1784,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>40</v>
       </c>
@@ -1794,7 +1807,7 @@
         <v>2.4062896219182036E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1817,7 +1830,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>80</v>
       </c>
@@ -1840,7 +1853,7 @@
         <v>5.5184762044969945E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1863,7 +1876,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>160</v>
       </c>
@@ -1886,7 +1899,7 @@
         <v>3.3344567242972914E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1909,7 +1922,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>320</v>
       </c>
@@ -1932,7 +1945,7 @@
         <v>2.4788591430648786E-5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1955,7 +1968,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>640</v>
       </c>
@@ -1978,7 +1991,7 @@
         <v>1.9207304432198693E-5</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -1989,7 +2002,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -2012,7 +2025,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>10</v>
       </c>
@@ -2035,7 +2048,7 @@
         <v>5.8181439485113203E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -2058,7 +2071,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>20</v>
       </c>
@@ -2081,7 +2094,7 @@
         <v>5.5956836342168552E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -2104,7 +2117,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>40</v>
       </c>
@@ -2127,7 +2140,7 @@
         <v>5.2508146184108607E-5</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -2150,7 +2163,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>80</v>
       </c>
@@ -2173,7 +2186,7 @@
         <v>5.2423183736345643E-6</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -2196,7 +2209,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>160</v>
       </c>
@@ -2219,7 +2232,7 @@
         <v>5.6835285441281644E-7</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -2242,7 +2255,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>320</v>
       </c>
@@ -2265,7 +2278,7 @@
         <v>6.5677249042175759E-8</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>0</v>
       </c>
@@ -2288,7 +2301,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>640</v>
       </c>
@@ -2311,7 +2324,7 @@
         <v>7.8902039692401263E-9</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>8</v>
       </c>
@@ -2322,7 +2335,7 @@
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>0</v>
       </c>
@@ -2345,7 +2358,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>10</v>
       </c>
@@ -2368,7 +2381,7 @@
         <v>3.4630229389760641E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -2391,7 +2404,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>20</v>
       </c>
@@ -2414,7 +2427,7 @@
         <v>3.5109658310429717E-4</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>0</v>
       </c>
@@ -2437,7 +2450,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>40</v>
       </c>
@@ -2460,7 +2473,7 @@
         <v>3.8235961059241184E-5</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>0</v>
       </c>
@@ -2483,7 +2496,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>80</v>
       </c>
@@ -2506,7 +2519,7 @@
         <v>4.4737432019519417E-6</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>0</v>
       </c>
@@ -2529,7 +2542,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>160</v>
       </c>
@@ -2552,7 +2565,7 @@
         <v>5.4370071135308591E-7</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>0</v>
       </c>
@@ -2575,7 +2588,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>320</v>
       </c>
@@ -2598,7 +2611,7 @@
         <v>6.6991104185819468E-8</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>0</v>
       </c>
@@ -2621,7 +2634,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>640</v>
       </c>
@@ -2642,6 +2655,328 @@
       </c>
       <c r="G62">
         <v>8.1938332455475691E-9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" t="s">
+        <v>2</v>
+      </c>
+      <c r="D64" t="s">
+        <v>3</v>
+      </c>
+      <c r="E64" t="s">
+        <v>4</v>
+      </c>
+      <c r="F64" t="s">
+        <v>5</v>
+      </c>
+      <c r="G64" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>10</v>
+      </c>
+      <c r="B65">
+        <v>5.5325644067524826E-3</v>
+      </c>
+      <c r="C65">
+        <v>8.1358744113576281E-3</v>
+      </c>
+      <c r="D65">
+        <v>1.0137008744486919E-2</v>
+      </c>
+      <c r="E65">
+        <v>6.0554303718530402E-3</v>
+      </c>
+      <c r="F65">
+        <v>7.0835529176820344E-3</v>
+      </c>
+      <c r="G65">
+        <v>2.5343750341119404E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>0</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1</v>
+      </c>
+      <c r="C67" t="s">
+        <v>2</v>
+      </c>
+      <c r="D67" t="s">
+        <v>3</v>
+      </c>
+      <c r="E67" t="s">
+        <v>4</v>
+      </c>
+      <c r="F67" t="s">
+        <v>5</v>
+      </c>
+      <c r="G67" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>20</v>
+      </c>
+      <c r="B68">
+        <v>1.5932184554642292E-3</v>
+      </c>
+      <c r="C68">
+        <v>1.882061543581367E-3</v>
+      </c>
+      <c r="D68">
+        <v>2.3427203569124089E-3</v>
+      </c>
+      <c r="E68">
+        <v>1.3775279362177627E-3</v>
+      </c>
+      <c r="F68">
+        <v>9.5690421308780582E-4</v>
+      </c>
+      <c r="G68">
+        <v>2.9468542530455377E-4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>0</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s">
+        <v>2</v>
+      </c>
+      <c r="D70" t="s">
+        <v>3</v>
+      </c>
+      <c r="E70" t="s">
+        <v>4</v>
+      </c>
+      <c r="F70" t="s">
+        <v>5</v>
+      </c>
+      <c r="G70" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>40</v>
+      </c>
+      <c r="B71">
+        <v>4.3282804144739728E-4</v>
+      </c>
+      <c r="C71">
+        <v>4.4311111741686632E-4</v>
+      </c>
+      <c r="D71">
+        <v>5.7010028636683696E-4</v>
+      </c>
+      <c r="E71">
+        <v>3.341127930681821E-4</v>
+      </c>
+      <c r="F71">
+        <v>1.2568529715106802E-4</v>
+      </c>
+      <c r="G71">
+        <v>3.5707464396554837E-5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>0</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1</v>
+      </c>
+      <c r="C73" t="s">
+        <v>2</v>
+      </c>
+      <c r="D73" t="s">
+        <v>3</v>
+      </c>
+      <c r="E73" t="s">
+        <v>4</v>
+      </c>
+      <c r="F73" t="s">
+        <v>5</v>
+      </c>
+      <c r="G73" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>80</v>
+      </c>
+      <c r="B74">
+        <v>1.14338234521838E-4</v>
+      </c>
+      <c r="C74">
+        <v>1.0555446270571588E-4</v>
+      </c>
+      <c r="D74">
+        <v>1.4132591989657328E-4</v>
+      </c>
+      <c r="E74">
+        <v>8.2552228037953489E-5</v>
+      </c>
+      <c r="F74">
+        <v>1.6151293232846697E-5</v>
+      </c>
+      <c r="G74">
+        <v>4.4027396481681386E-6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>0</v>
+      </c>
+      <c r="B76" t="s">
+        <v>1</v>
+      </c>
+      <c r="C76" t="s">
+        <v>2</v>
+      </c>
+      <c r="D76" t="s">
+        <v>3</v>
+      </c>
+      <c r="E76" t="s">
+        <v>4</v>
+      </c>
+      <c r="F76" t="s">
+        <v>5</v>
+      </c>
+      <c r="G76" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>160</v>
+      </c>
+      <c r="B77">
+        <v>2.9740733296479416E-5</v>
+      </c>
+      <c r="C77">
+        <v>2.5353481101861328E-5</v>
+      </c>
+      <c r="D77">
+        <v>3.5231553889236711E-5</v>
+      </c>
+      <c r="E77">
+        <v>2.0530821332468879E-5</v>
+      </c>
+      <c r="F77">
+        <v>2.0485420385019104E-6</v>
+      </c>
+      <c r="G77">
+        <v>5.4686457700125853E-7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>0</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1</v>
+      </c>
+      <c r="C79" t="s">
+        <v>2</v>
+      </c>
+      <c r="D79" t="s">
+        <v>3</v>
+      </c>
+      <c r="E79" t="s">
+        <v>4</v>
+      </c>
+      <c r="F79" t="s">
+        <v>5</v>
+      </c>
+      <c r="G79" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>320</v>
+      </c>
+      <c r="B80">
+        <v>7.6630776562613967E-6</v>
+      </c>
+      <c r="C80">
+        <v>6.1289099365040553E-6</v>
+      </c>
+      <c r="D80">
+        <v>8.7987684685986167E-6</v>
+      </c>
+      <c r="E80">
+        <v>5.1200972594610432E-6</v>
+      </c>
+      <c r="F80">
+        <v>2.5799405012350007E-7</v>
+      </c>
+      <c r="G80">
+        <v>6.8151931438667817E-8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>0</v>
+      </c>
+      <c r="B82" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82" t="s">
+        <v>2</v>
+      </c>
+      <c r="D82" t="s">
+        <v>3</v>
+      </c>
+      <c r="E82" t="s">
+        <v>4</v>
+      </c>
+      <c r="F82" t="s">
+        <v>5</v>
+      </c>
+      <c r="G82" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>640</v>
+      </c>
+      <c r="B83">
+        <v>1.9619930370362582E-6</v>
+      </c>
+      <c r="C83">
+        <v>1.4893639266766234E-6</v>
+      </c>
+      <c r="D83">
+        <v>2.1988049006549382E-6</v>
+      </c>
+      <c r="E83">
+        <v>1.2784948175415629E-6</v>
+      </c>
+      <c r="F83">
+        <v>3.237276324785654E-8</v>
+      </c>
+      <c r="G83">
+        <v>8.5067045532944261E-9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>